<commit_message>
Update 28. Dashboards Impressionadores
Anotações e Prática. Aulas da 18 à 21.
</commit_message>
<xml_diff>
--- a/28. Dashboards Impressionadores/Dashboards Impressionadores - Caixa de Combinação - Dashboards Impressionadores - Pasta de Trabalho 5.xlsx
+++ b/28. Dashboards Impressionadores/Dashboards Impressionadores - Caixa de Combinação - Dashboards Impressionadores - Pasta de Trabalho 5.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kiko\Documents\Projetos Programação\Especializacao-em-Analise-de-Dados\28. Dashboards Impressionadores\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66488D68-63DB-4C17-8186-C3625032AC8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{549236B5-9201-418B-A9D3-E3792AD019AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="982" activeTab="3" xr2:uid="{A0D6CE5D-8462-400E-B7A6-65CA78D18720}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="982" firstSheet="5" activeTab="11" xr2:uid="{A0D6CE5D-8462-400E-B7A6-65CA78D18720}"/>
   </bookViews>
   <sheets>
     <sheet name="Caixa de Combinação" sheetId="2" r:id="rId1"/>
@@ -27,6 +27,14 @@
     <sheet name="Botão de Opção (Prática)" sheetId="17" r:id="rId12"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">'Botão de Rotação (Prática)'!$B$8:$E$8</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">'Botão de Rotação (Prática)'!$I$3:$L$3</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">'Botão de Rotação (Prática)'!$I$4:$L$4</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">'Botão de Rotação (Prática)'!$I$5:$L$5</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">'Botão de Rotação (Prática)'!$B$8:$E$8</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">'Botão de Rotação (Prática)'!$I$3:$L$3</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">'Botão de Rotação (Prática)'!$B$8:$E$8</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">'Botão de Rotação (Prática)'!$I$3:$L$3</definedName>
     <definedName name="Pos_1">INDEX(#REF!,MATCH(#REF!,#REF!,0))</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -70,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="26">
   <si>
     <t>Marca A</t>
   </si>
@@ -143,6 +151,12 @@
   <si>
     <t>Valores retorno</t>
   </si>
+  <si>
+    <t>&lt;=</t>
+  </si>
+  <si>
+    <t>QUAL MELHOR PROFESSOR ??</t>
+  </si>
 </sst>
 </file>
 
@@ -152,7 +166,7 @@
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="&quot;R$&quot;\ #,##0"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -186,8 +200,13 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -224,6 +243,17 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF57FFA3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -245,12 +275,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -310,22 +341,59 @@
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="43" fontId="0" fillId="8" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="43" fontId="0" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="2" fillId="7" borderId="0" xfId="3" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
+    <cellStyle name="Ênfase1" xfId="3" builtinId="29"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Porcentagem" xfId="1" builtinId="5"/>
     <cellStyle name="Vírgula" xfId="2" builtinId="3"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="11">
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor rgb="FFFF7575"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
+        <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="7"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF57FFA3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFB7B7"/>
         </patternFill>
       </fill>
     </dxf>
@@ -344,30 +412,14 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
       <fill>
         <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF57FFA3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFB7B7"/>
+          <bgColor theme="7"/>
         </patternFill>
       </fill>
     </dxf>
@@ -399,10 +451,10 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFF7575"/>
+      <color rgb="FF57FFA3"/>
+      <color rgb="FF75FFB3"/>
       <color rgb="FFFFB7B7"/>
-      <color rgb="FF57FFA3"/>
-      <color rgb="FFFF7575"/>
-      <color rgb="FF75FFB3"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1118,7 +1170,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>68371</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1189,7 +1241,7 @@
                   <c:v>20327</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>68371</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1365,16 +1417,16 @@
                 <c:formatCode>"R$"\ #,##0</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>60000</c:v>
+                  <c:v>70000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>60000</c:v>
+                  <c:v>70000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>60000</c:v>
+                  <c:v>70000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>60000</c:v>
+                  <c:v>70000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1487,6 +1539,358 @@
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Maior</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="57FFA3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'Botão de Rotação (Prática)'!$I$4:$L$4</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>98413</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-8534-465E-A07F-EC0372CB7E27}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Menor</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FF7575"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'Botão de Rotação (Prática)'!$I$5:$L$5</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>81678</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>72793</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>85934</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-8534-465E-A07F-EC0372CB7E27}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="100"/>
+        <c:axId val="9939167"/>
+        <c:axId val="9925247"/>
+      </c:barChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Linha</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="dash"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Botão de Rotação (Prática)'!$B$8:$E$8</c:f>
+              <c:numCache>
+                <c:formatCode>"R$"\ #,##0</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>90000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>90000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>90000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>90000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Botão de Rotação (Prática)'!$B$8:$E$8</c:f>
+              <c:numCache>
+                <c:formatCode>"R$"\ #,##0</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>90000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>90000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>90000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>90000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-8534-465E-A07F-EC0372CB7E27}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="9939167"/>
+        <c:axId val="9925247"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="9939167"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="&quot;R$&quot;\ #,##0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="9925247"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="9925247"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="9939167"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
       <a:round/>
     </a:ln>
     <a:effectLst/>
@@ -1629,6 +2033,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -3140,48 +3584,551 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropStyle="combo" dx="26" fmlaLink="$J$2" fmlaRange="$A$2:$A$7" noThreeD="1" sel="2" val="0"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp10.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="26" fmlaLink="$H$6" max="10" min="1" page="10" val="9"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp11.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="26" fmlaLink="$I$2" horiz="1" max="100" page="10" val="80"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp12.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="26" fmlaLink="$H$2" horiz="1" max="100" page="10" val="68"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp13.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$B$2" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp14.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$B$3" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp15.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$B$4" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp16.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$B$5" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp14.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$B$6" lockText="1" noThreeD="1"/>
+<file path=xl/ctrlProps/ctrlProp17.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$B$6" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp18.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$B$7" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp19.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$B$8" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp17.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$B$9" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp18.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$B$10" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp19.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$B$11" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3189,39 +4136,107 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp20.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="GBox"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$B$9" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp21.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Radio" firstButton="1" fmlaLink="$I$2" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$B$10" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp22.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Radio" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$B$11" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp23.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Radio" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$D$2" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp24.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Radio" checked="Checked" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$D$3" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp25.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Radio" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$D$4" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp26.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Label" lockText="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$D$5" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp27.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$D$6" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp28.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$D$7" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp29.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$D$8" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="List" dx="26" fmlaLink="$K$2" fmlaRange="$A$2:$A$25" sel="6" val="0"/>
 </file>
 
+<file path=xl/ctrlProps/ctrlProp30.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$D$9" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp31.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$D$10" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp32.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$D$11" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp33.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="GBox"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp34.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Radio" firstButton="1" fmlaLink="$I$2" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp35.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Radio" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp36.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Radio" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp37.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Radio" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp38.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Radio" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp39.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Label" lockText="1"/>
+</file>
+
 <file path=xl/ctrlProps/ctrlProp4.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="List" dx="26" fmlaLink="$M$7" fmlaRange="$M$2:$M$5" sel="4" val="0"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp40.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Radio" firstButton="1" fmlaLink="$F$2" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp41.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Radio" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp42.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Radio" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp43.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Radio" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp5.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3237,11 +4252,11 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp8.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="26" fmlaLink="$H$1" max="10" page="10" val="6"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="26" fmlaLink="$H$1" max="10" page="10" val="7"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp9.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="26" fmlaLink="$I$2" horiz="1" max="100" page="10" val="70"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropStyle="combo" dx="26" fmlaLink="$H$2" fmlaRange="$A$2:$A$7" sel="1" val="0"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3487,6 +4502,1604 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing10.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>598805</xdr:colOff>
+          <xdr:row>0</xdr:row>
+          <xdr:rowOff>158750</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>987425</xdr:colOff>
+          <xdr:row>2</xdr:row>
+          <xdr:rowOff>12700</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="22529" name="Check Box 1" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s22529"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0900-000001580000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>598805</xdr:colOff>
+          <xdr:row>1</xdr:row>
+          <xdr:rowOff>159597</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>987425</xdr:colOff>
+          <xdr:row>3</xdr:row>
+          <xdr:rowOff>13547</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="22530" name="Check Box 2" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s22530"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{67889EEF-BDB2-3384-9A15-CC01A0ACBEDD}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>598805</xdr:colOff>
+          <xdr:row>2</xdr:row>
+          <xdr:rowOff>160444</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>987425</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>14394</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="22531" name="Check Box 3" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s22531"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D4297C2D-EE4E-61CB-0859-4978F9DEA2FA}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>598805</xdr:colOff>
+          <xdr:row>3</xdr:row>
+          <xdr:rowOff>161291</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>987425</xdr:colOff>
+          <xdr:row>5</xdr:row>
+          <xdr:rowOff>15241</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="22532" name="Check Box 4" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s22532"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D1A30321-CE76-1912-C08F-7635D81AA4CE}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>598805</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>162138</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>987425</xdr:colOff>
+          <xdr:row>6</xdr:row>
+          <xdr:rowOff>16088</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="22535" name="Check Box 7" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s22535"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6DD0169A-B6D3-CA00-7081-EA38E60FA6DA}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>598805</xdr:colOff>
+          <xdr:row>5</xdr:row>
+          <xdr:rowOff>162985</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>987425</xdr:colOff>
+          <xdr:row>7</xdr:row>
+          <xdr:rowOff>16935</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="22536" name="Check Box 8" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s22536"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{17E61BF9-4E02-B987-DC82-896EFF57167B}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>598805</xdr:colOff>
+          <xdr:row>6</xdr:row>
+          <xdr:rowOff>163832</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>987425</xdr:colOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>17782</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="22537" name="Check Box 9" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s22537"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{74FF2599-4F52-6351-56D1-BF91C8B4D737}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>598805</xdr:colOff>
+          <xdr:row>7</xdr:row>
+          <xdr:rowOff>164679</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>987425</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>18629</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="22538" name="Check Box 10" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s22538"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4AA0339A-3129-8D26-3236-7479E020CF4C}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>598805</xdr:colOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>165526</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>987425</xdr:colOff>
+          <xdr:row>10</xdr:row>
+          <xdr:rowOff>19476</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="22539" name="Check Box 11" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s22539"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{86DC089E-95CF-2926-A869-49DB56C20A3F}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>598805</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>166370</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>987425</xdr:colOff>
+          <xdr:row>11</xdr:row>
+          <xdr:rowOff>20320</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="22540" name="Check Box 12" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s22540"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{39BD3FAE-83AF-EFFF-FE49-2F08A126319A}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing11.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>1</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>7</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>60960</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="8195" name="Group Box 3" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s8195"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0A00-000003200000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:noFill/>
+                </a14:hiddenFill>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>91440</xdr:colOff>
+          <xdr:row>2</xdr:row>
+          <xdr:rowOff>106680</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>388620</xdr:colOff>
+          <xdr:row>3</xdr:row>
+          <xdr:rowOff>144780</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="8196" name="Option Button 4" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s8196"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0A00-000004200000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="0" bIns="27432" anchor="ctr" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="pt-BR" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Segoe UI"/>
+                  <a:cs typeface="Segoe UI"/>
+                </a:rPr>
+                <a:t>João Martins</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>91440</xdr:colOff>
+          <xdr:row>3</xdr:row>
+          <xdr:rowOff>114300</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>388620</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>152400</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="8197" name="Option Button 5" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s8197"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0A00-000005200000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="0" bIns="27432" anchor="ctr" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="pt-BR" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Segoe UI"/>
+                  <a:cs typeface="Segoe UI"/>
+                </a:rPr>
+                <a:t>Alon Pinheiro</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>91440</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>129540</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>388620</xdr:colOff>
+          <xdr:row>5</xdr:row>
+          <xdr:rowOff>167640</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="8198" name="Option Button 6" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s8198"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0A00-000006200000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="0" bIns="27432" anchor="ctr" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="pt-BR" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Segoe UI"/>
+                  <a:cs typeface="Segoe UI"/>
+                </a:rPr>
+                <a:t>Diego Amorim</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>91440</xdr:colOff>
+          <xdr:row>5</xdr:row>
+          <xdr:rowOff>137160</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>388620</xdr:colOff>
+          <xdr:row>6</xdr:row>
+          <xdr:rowOff>175260</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="8199" name="Option Button 7" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s8199"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0A00-000007200000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="0" bIns="27432" anchor="ctr" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="pt-BR" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Segoe UI"/>
+                  <a:cs typeface="Segoe UI"/>
+                </a:rPr>
+                <a:t>Marcus Cavalcanti</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>91440</xdr:colOff>
+          <xdr:row>6</xdr:row>
+          <xdr:rowOff>144780</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>388620</xdr:colOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="8200" name="Option Button 8" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s8200"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0A00-000008200000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="0" bIns="27432" anchor="ctr" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="pt-BR" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Segoe UI"/>
+                  <a:cs typeface="Segoe UI"/>
+                </a:rPr>
+                <a:t>João Lira</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor>
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>114300</xdr:colOff>
+          <xdr:row>1</xdr:row>
+          <xdr:rowOff>83820</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>350520</xdr:colOff>
+          <xdr:row>2</xdr:row>
+          <xdr:rowOff>121920</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="8201" name="Label 9" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s8201"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0A00-000009200000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:noFill/>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="0" bIns="0" anchor="t" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="pt-BR" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Segoe UI"/>
+                  <a:cs typeface="Segoe UI"/>
+                </a:rPr>
+                <a:t>Qual melhor professor da Hashtag?</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing12.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>2</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>1219200</xdr:colOff>
+          <xdr:row>3</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="23553" name="Option Button 1" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s23553"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0B00-0000015C0000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="32004" rIns="0" bIns="32004" anchor="ctr" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="pt-BR" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Segoe UI"/>
+                  <a:cs typeface="Segoe UI"/>
+                </a:rPr>
+                <a:t>João</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>3</xdr:row>
+          <xdr:rowOff>6350</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>1219200</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>6350</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="23554" name="Option Button 2" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s23554"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5A6AD6E5-234D-D9A1-F0F4-6ADF157191D3}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="32004" rIns="0" bIns="32004" anchor="ctr" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="pt-BR" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Segoe UI"/>
+                  <a:cs typeface="Segoe UI"/>
+                </a:rPr>
+                <a:t>Alon</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>1219200</xdr:colOff>
+          <xdr:row>5</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="23555" name="Option Button 3" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s23555"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{779B9EE4-FDB3-8B98-E3A4-6E6D3E2FEC37}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="32004" rIns="0" bIns="32004" anchor="ctr" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="pt-BR" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Segoe UI"/>
+                  <a:cs typeface="Segoe UI"/>
+                </a:rPr>
+                <a:t>Marcus</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>5</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>1219200</xdr:colOff>
+          <xdr:row>6</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="23556" name="Option Button 4" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s23556"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{823B666C-5BD1-6353-7567-AC71C7AE440E}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="32004" rIns="0" bIns="32004" anchor="ctr" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="pt-BR" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Segoe UI"/>
+                  <a:cs typeface="Segoe UI"/>
+                </a:rPr>
+                <a:t>Diego</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+</xdr:wsDr>
+</file>
+
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -3496,13 +6109,13 @@
           <xdr:col>6</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>0</xdr:row>
-          <xdr:rowOff>88900</xdr:rowOff>
+          <xdr:rowOff>91440</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>12</xdr:col>
           <xdr:colOff>228600</xdr:colOff>
           <xdr:row>1</xdr:row>
-          <xdr:rowOff>88900</xdr:rowOff>
+          <xdr:rowOff>91440</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3714,15 +6327,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>7</xdr:col>
-          <xdr:colOff>217170</xdr:colOff>
+          <xdr:colOff>220980</xdr:colOff>
           <xdr:row>0</xdr:row>
-          <xdr:rowOff>80010</xdr:rowOff>
+          <xdr:rowOff>83820</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>8</xdr:col>
-          <xdr:colOff>488950</xdr:colOff>
+          <xdr:colOff>487680</xdr:colOff>
           <xdr:row>11</xdr:row>
-          <xdr:rowOff>88900</xdr:rowOff>
+          <xdr:rowOff>91440</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3772,15 +6385,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>9</xdr:col>
-          <xdr:colOff>55880</xdr:colOff>
+          <xdr:colOff>53340</xdr:colOff>
           <xdr:row>0</xdr:row>
-          <xdr:rowOff>87630</xdr:rowOff>
+          <xdr:rowOff>91440</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>10</xdr:col>
-          <xdr:colOff>322580</xdr:colOff>
+          <xdr:colOff>320040</xdr:colOff>
           <xdr:row>11</xdr:row>
-          <xdr:rowOff>95250</xdr:rowOff>
+          <xdr:rowOff>99060</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3790,7 +6403,7 @@
                   <a14:compatExt spid="_x0000_s14339"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9570DAD0-BFCA-286E-A76A-191FB2559FFB}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003380000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4128,6 +6741,155 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
+          <xdr:colOff>13970</xdr:colOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>133350</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>158750</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>153670</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="20481" name="Drop Down 1" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s20481"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000001500000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>482600</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{905CE6E3-09B6-7CFF-3D7C-0350B2D899CA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor>
+        <xdr:from>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>7</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="20482" name="Spinner 2" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s20482"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000002500000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>1</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
@@ -4176,7 +6938,62 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>12700</xdr:colOff>
+          <xdr:row>0</xdr:row>
+          <xdr:rowOff>168910</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>3</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="21505" name="Scroll Bar 1" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s21505"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000001540000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
@@ -4851,580 +7668,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>1</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
-          <xdr:row>1</xdr:row>
-          <xdr:rowOff>0</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>7</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
-          <xdr:row>8</xdr:row>
-          <xdr:rowOff>60960</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="8195" name="Group Box 3" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s8195"/>
-                </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0A00-000003200000}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln w="9525">
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:noFill/>
-                </a14:hiddenFill>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>1</xdr:col>
-          <xdr:colOff>91440</xdr:colOff>
-          <xdr:row>2</xdr:row>
-          <xdr:rowOff>106680</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>3</xdr:col>
-          <xdr:colOff>388620</xdr:colOff>
-          <xdr:row>3</xdr:row>
-          <xdr:rowOff>144780</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="8196" name="Option Button 4" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s8196"/>
-                </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0A00-000004200000}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="0" bIns="27432" anchor="ctr" upright="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="l" rtl="0">
-                <a:defRPr sz="1000"/>
-              </a:pPr>
-              <a:r>
-                <a:rPr lang="pt-BR" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                  <a:solidFill>
-                    <a:srgbClr val="000000"/>
-                  </a:solidFill>
-                  <a:latin typeface="Segoe UI"/>
-                  <a:cs typeface="Segoe UI"/>
-                </a:rPr>
-                <a:t>João Martins</a:t>
-              </a:r>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>1</xdr:col>
-          <xdr:colOff>91440</xdr:colOff>
-          <xdr:row>3</xdr:row>
-          <xdr:rowOff>114300</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>3</xdr:col>
-          <xdr:colOff>388620</xdr:colOff>
-          <xdr:row>4</xdr:row>
-          <xdr:rowOff>152400</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="8197" name="Option Button 5" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s8197"/>
-                </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0A00-000005200000}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="0" bIns="27432" anchor="ctr" upright="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="l" rtl="0">
-                <a:defRPr sz="1000"/>
-              </a:pPr>
-              <a:r>
-                <a:rPr lang="pt-BR" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                  <a:solidFill>
-                    <a:srgbClr val="000000"/>
-                  </a:solidFill>
-                  <a:latin typeface="Segoe UI"/>
-                  <a:cs typeface="Segoe UI"/>
-                </a:rPr>
-                <a:t>Alon Pinheiro</a:t>
-              </a:r>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>1</xdr:col>
-          <xdr:colOff>91440</xdr:colOff>
-          <xdr:row>4</xdr:row>
-          <xdr:rowOff>129540</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>3</xdr:col>
-          <xdr:colOff>388620</xdr:colOff>
-          <xdr:row>5</xdr:row>
-          <xdr:rowOff>167640</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="8198" name="Option Button 6" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s8198"/>
-                </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0A00-000006200000}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="0" bIns="27432" anchor="ctr" upright="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="l" rtl="0">
-                <a:defRPr sz="1000"/>
-              </a:pPr>
-              <a:r>
-                <a:rPr lang="pt-BR" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                  <a:solidFill>
-                    <a:srgbClr val="000000"/>
-                  </a:solidFill>
-                  <a:latin typeface="Segoe UI"/>
-                  <a:cs typeface="Segoe UI"/>
-                </a:rPr>
-                <a:t>Diego Amorim</a:t>
-              </a:r>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>1</xdr:col>
-          <xdr:colOff>91440</xdr:colOff>
-          <xdr:row>5</xdr:row>
-          <xdr:rowOff>137160</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>3</xdr:col>
-          <xdr:colOff>388620</xdr:colOff>
-          <xdr:row>6</xdr:row>
-          <xdr:rowOff>175260</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="8199" name="Option Button 7" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s8199"/>
-                </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0A00-000007200000}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="0" bIns="27432" anchor="ctr" upright="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="l" rtl="0">
-                <a:defRPr sz="1000"/>
-              </a:pPr>
-              <a:r>
-                <a:rPr lang="pt-BR" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                  <a:solidFill>
-                    <a:srgbClr val="000000"/>
-                  </a:solidFill>
-                  <a:latin typeface="Segoe UI"/>
-                  <a:cs typeface="Segoe UI"/>
-                </a:rPr>
-                <a:t>Marcus Cavalcanti</a:t>
-              </a:r>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>1</xdr:col>
-          <xdr:colOff>91440</xdr:colOff>
-          <xdr:row>6</xdr:row>
-          <xdr:rowOff>144780</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>3</xdr:col>
-          <xdr:colOff>388620</xdr:colOff>
-          <xdr:row>8</xdr:row>
-          <xdr:rowOff>0</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="8200" name="Option Button 8" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s8200"/>
-                </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0A00-000008200000}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="0" bIns="27432" anchor="ctr" upright="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="l" rtl="0">
-                <a:defRPr sz="1000"/>
-              </a:pPr>
-              <a:r>
-                <a:rPr lang="pt-BR" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                  <a:solidFill>
-                    <a:srgbClr val="000000"/>
-                  </a:solidFill>
-                  <a:latin typeface="Segoe UI"/>
-                  <a:cs typeface="Segoe UI"/>
-                </a:rPr>
-                <a:t>João Lira</a:t>
-              </a:r>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor>
-        <xdr:from>
-          <xdr:col>1</xdr:col>
-          <xdr:colOff>114300</xdr:colOff>
-          <xdr:row>1</xdr:row>
-          <xdr:rowOff>83820</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>4</xdr:col>
-          <xdr:colOff>350520</xdr:colOff>
-          <xdr:row>2</xdr:row>
-          <xdr:rowOff>121920</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="8201" name="Label 9" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s8201"/>
-                </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0A00-000009200000}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:noFill/>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:noFill/>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="0" bIns="0" anchor="t" upright="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="l" rtl="0">
-                <a:defRPr sz="1000"/>
-              </a:pPr>
-              <a:r>
-                <a:rPr lang="pt-BR" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                  <a:solidFill>
-                    <a:srgbClr val="000000"/>
-                  </a:solidFill>
-                  <a:latin typeface="Segoe UI"/>
-                  <a:cs typeface="Segoe UI"/>
-                </a:rPr>
-                <a:t>Qual melhor professor da Hashtag?</a:t>
-              </a:r>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-</xdr:wsDr>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office 2013 - 2022">
   <a:themeElements>
@@ -5919,77 +8162,344 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC143E37-4E7A-443F-AF33-9B504BF56E09}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC143E37-4E7A-443F-AF33-9B504BF56E09}">
   <sheetPr>
     <tabColor theme="7"/>
   </sheetPr>
-  <dimension ref="A1:A11"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.5546875" customWidth="1"/>
+    <col min="4" max="4" width="12" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>22</v>
       </c>
+      <c r="D11" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="27">
+        <f>COUNTIFS(D2:D11,TRUE)/COUNTA(D2:D11)</f>
+        <v>0.5</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x14">
+      <controls>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="22529" r:id="rId3" name="Check Box 1">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>0</xdr:col>
+                    <xdr:colOff>601980</xdr:colOff>
+                    <xdr:row>0</xdr:row>
+                    <xdr:rowOff>160020</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>0</xdr:col>
+                    <xdr:colOff>990600</xdr:colOff>
+                    <xdr:row>2</xdr:row>
+                    <xdr:rowOff>15240</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="22530" r:id="rId4" name="Check Box 2">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>0</xdr:col>
+                    <xdr:colOff>601980</xdr:colOff>
+                    <xdr:row>1</xdr:row>
+                    <xdr:rowOff>160020</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>0</xdr:col>
+                    <xdr:colOff>990600</xdr:colOff>
+                    <xdr:row>3</xdr:row>
+                    <xdr:rowOff>15240</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="22531" r:id="rId5" name="Check Box 3">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>0</xdr:col>
+                    <xdr:colOff>601980</xdr:colOff>
+                    <xdr:row>2</xdr:row>
+                    <xdr:rowOff>160020</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>0</xdr:col>
+                    <xdr:colOff>990600</xdr:colOff>
+                    <xdr:row>4</xdr:row>
+                    <xdr:rowOff>15240</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="22532" r:id="rId6" name="Check Box 4">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>0</xdr:col>
+                    <xdr:colOff>601980</xdr:colOff>
+                    <xdr:row>3</xdr:row>
+                    <xdr:rowOff>160020</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>0</xdr:col>
+                    <xdr:colOff>990600</xdr:colOff>
+                    <xdr:row>5</xdr:row>
+                    <xdr:rowOff>15240</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="22535" r:id="rId7" name="Check Box 7">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>0</xdr:col>
+                    <xdr:colOff>601980</xdr:colOff>
+                    <xdr:row>4</xdr:row>
+                    <xdr:rowOff>160020</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>0</xdr:col>
+                    <xdr:colOff>990600</xdr:colOff>
+                    <xdr:row>6</xdr:row>
+                    <xdr:rowOff>15240</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="22536" r:id="rId8" name="Check Box 8">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>0</xdr:col>
+                    <xdr:colOff>601980</xdr:colOff>
+                    <xdr:row>5</xdr:row>
+                    <xdr:rowOff>160020</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>0</xdr:col>
+                    <xdr:colOff>990600</xdr:colOff>
+                    <xdr:row>7</xdr:row>
+                    <xdr:rowOff>15240</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="22537" r:id="rId9" name="Check Box 9">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>0</xdr:col>
+                    <xdr:colOff>601980</xdr:colOff>
+                    <xdr:row>6</xdr:row>
+                    <xdr:rowOff>167640</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>0</xdr:col>
+                    <xdr:colOff>990600</xdr:colOff>
+                    <xdr:row>8</xdr:row>
+                    <xdr:rowOff>15240</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="22538" r:id="rId10" name="Check Box 10">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>0</xdr:col>
+                    <xdr:colOff>601980</xdr:colOff>
+                    <xdr:row>7</xdr:row>
+                    <xdr:rowOff>167640</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>0</xdr:col>
+                    <xdr:colOff>990600</xdr:colOff>
+                    <xdr:row>9</xdr:row>
+                    <xdr:rowOff>15240</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="22539" r:id="rId11" name="Check Box 11">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>0</xdr:col>
+                    <xdr:colOff>601980</xdr:colOff>
+                    <xdr:row>8</xdr:row>
+                    <xdr:rowOff>167640</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>0</xdr:col>
+                    <xdr:colOff>990600</xdr:colOff>
+                    <xdr:row>10</xdr:row>
+                    <xdr:rowOff>22860</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="22540" r:id="rId12" name="Check Box 12">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>0</xdr:col>
+                    <xdr:colOff>601980</xdr:colOff>
+                    <xdr:row>9</xdr:row>
+                    <xdr:rowOff>167640</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>0</xdr:col>
+                    <xdr:colOff>990600</xdr:colOff>
+                    <xdr:row>11</xdr:row>
+                    <xdr:rowOff>22860</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+      </controls>
+    </mc:Choice>
+  </mc:AlternateContent>
 </worksheet>
 </file>
 
@@ -6017,10 +8527,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B10:G10">
-    <cfRule type="expression" dxfId="6" priority="1">
+    <cfRule type="expression" dxfId="4" priority="1">
       <formula>$I$2&lt;&gt;1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="2">
+    <cfRule type="expression" dxfId="3" priority="2">
       <formula>$I$2=1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6191,17 +8701,144 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7288C57E-27DB-40EE-8F46-9B1A716A90B2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7288C57E-27DB-40EE-8F46-9B1A716A90B2}">
   <sheetPr>
     <tabColor theme="7"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="B2:F8"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="26.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B8" s="8" t="str">
+        <f>IF(F2=2,"Professor certo","Professor errado")</f>
+        <v>Professor certo</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B8">
+    <cfRule type="expression" dxfId="0" priority="3">
+      <formula>"Professor errado"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>"Professor errado"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+      <formula>"Professor certo"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x14">
+      <controls>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="23553" r:id="rId3" name="Option Button 1">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:row>2</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>1219200</xdr:colOff>
+                    <xdr:row>3</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="23554" r:id="rId4" name="Option Button 2">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:row>3</xdr:row>
+                    <xdr:rowOff>7620</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>1219200</xdr:colOff>
+                    <xdr:row>4</xdr:row>
+                    <xdr:rowOff>7620</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="23555" r:id="rId5" name="Option Button 3">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:row>4</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>1219200</xdr:colOff>
+                    <xdr:row>5</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="23556" r:id="rId6" name="Option Button 4">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:row>5</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>1219200</xdr:colOff>
+                    <xdr:row>6</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+      </controls>
+    </mc:Choice>
+  </mc:AlternateContent>
 </worksheet>
 </file>
 
@@ -6890,13 +9527,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:E25">
-    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
       <formula>$O$2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="2">
+    <cfRule type="expression" dxfId="9" priority="2">
       <formula>B$1=$M$8</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="5">
+    <cfRule type="expression" dxfId="8" priority="5">
       <formula>$A2=$K$3</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6963,7 +9600,7 @@
   </sheetPr>
   <dimension ref="A1:O25"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
@@ -7436,41 +10073,21 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:B25">
-    <cfRule type="expression" priority="9">
+  <conditionalFormatting sqref="B2:E25">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
+      <formula>$M$4</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="6" priority="2">
+      <formula>$A2=$M$2</formula>
+    </cfRule>
+    <cfRule type="expression" priority="3">
+      <formula>$A2=$M$2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="5" priority="6">
       <formula>B$1=$M$3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="8">
+    <cfRule type="expression" priority="7">
       <formula>B$1=$M$3</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C2:E25">
-    <cfRule type="expression" dxfId="3" priority="6">
-      <formula>C$1=$M$3</formula>
-    </cfRule>
-    <cfRule type="expression" priority="7">
-      <formula>C$1=$M$3</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B2:E2">
-    <cfRule type="expression" priority="5">
-      <formula>$A2=$M$2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="2" priority="4">
-      <formula>$A2=$M$2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B3:E25">
-    <cfRule type="expression" dxfId="1" priority="2">
-      <formula>$A3=$M$2</formula>
-    </cfRule>
-    <cfRule type="expression" priority="3">
-      <formula>$A3=$M$2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B2:E25">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
-      <formula>$M$4</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -7562,7 +10179,7 @@
       </c>
       <c r="F1" s="1"/>
       <c r="H1" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
@@ -7584,7 +10201,7 @@
       <c r="F2" s="1"/>
       <c r="H2" s="1">
         <f>H1*10000</f>
-        <v>60000</v>
+        <v>70000</v>
       </c>
       <c r="J2" s="1">
         <v>4</v>
@@ -7662,7 +10279,7 @@
       </c>
       <c r="N4" s="3">
         <f t="shared" si="0"/>
-        <v>68371</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
@@ -7699,7 +10316,7 @@
       </c>
       <c r="N5" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>68371</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
@@ -7744,19 +10361,19 @@
       </c>
       <c r="B8" s="10">
         <f>$H$2</f>
-        <v>60000</v>
+        <v>70000</v>
       </c>
       <c r="C8" s="10">
         <f t="shared" ref="C8:E8" si="2">$H$2</f>
-        <v>60000</v>
+        <v>70000</v>
       </c>
       <c r="D8" s="10">
         <f t="shared" si="2"/>
-        <v>60000</v>
+        <v>70000</v>
       </c>
       <c r="E8" s="10">
         <f t="shared" si="2"/>
-        <v>60000</v>
+        <v>70000</v>
       </c>
       <c r="F8" s="1"/>
     </row>
@@ -7818,22 +10435,25 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{993D4F5B-6DFD-4112-8702-1C73E0E174DF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{993D4F5B-6DFD-4112-8702-1C73E0E174DF}">
   <sheetPr>
     <tabColor theme="7"/>
   </sheetPr>
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="7.33203125" customWidth="1"/>
     <col min="2" max="5" width="12.21875" customWidth="1"/>
     <col min="6" max="6" width="7.21875" customWidth="1"/>
+    <col min="9" max="12" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>4</v>
       </c>
@@ -7851,7 +10471,7 @@
       </c>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="9">
         <v>2015</v>
       </c>
@@ -7868,8 +10488,23 @@
         <v>98413</v>
       </c>
       <c r="F2" s="1"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="9">
         <v>2016</v>
       </c>
@@ -7886,8 +10521,28 @@
         <v>49048</v>
       </c>
       <c r="F3" s="1"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H3" cm="1">
+        <f t="array" ref="H3">INDEX(A2:A7,$H$2)</f>
+        <v>2015</v>
+      </c>
+      <c r="I3" s="20" cm="1">
+        <f t="array" ref="I3">INDEX(B2:B7,$H$2)</f>
+        <v>81678</v>
+      </c>
+      <c r="J3" s="20" cm="1">
+        <f t="array" ref="J3">INDEX(C2:C7,$H$2)</f>
+        <v>72793</v>
+      </c>
+      <c r="K3" s="20" cm="1">
+        <f t="array" ref="K3">INDEX(D2:D7,$H$2)</f>
+        <v>85934</v>
+      </c>
+      <c r="L3" s="20" cm="1">
+        <f t="array" ref="L3">INDEX(E2:E7,$H$2)</f>
+        <v>98413</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="9">
         <v>2017</v>
       </c>
@@ -7904,8 +10559,27 @@
         <v>60197</v>
       </c>
       <c r="F4" s="1"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H4" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="I4" s="24">
+        <f>IF(I3&gt;=$H$7,I3,0)</f>
+        <v>0</v>
+      </c>
+      <c r="J4" s="24">
+        <f t="shared" ref="J4:L4" si="0">IF(J3&gt;=$H$7,J3,0)</f>
+        <v>0</v>
+      </c>
+      <c r="K4" s="24">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L4" s="24">
+        <f t="shared" si="0"/>
+        <v>98413</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="9">
         <v>2018</v>
       </c>
@@ -7922,8 +10596,27 @@
         <v>68371</v>
       </c>
       <c r="F5" s="1"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H5" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="I5" s="26">
+        <f>IF(I3&lt;=$H$7,I3,0)</f>
+        <v>81678</v>
+      </c>
+      <c r="J5" s="26">
+        <f t="shared" ref="J5:L5" si="1">IF(J3&lt;=$H$7,J3,0)</f>
+        <v>72793</v>
+      </c>
+      <c r="K5" s="26">
+        <f t="shared" si="1"/>
+        <v>85934</v>
+      </c>
+      <c r="L5" s="26">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="9">
         <v>2019</v>
       </c>
@@ -7940,8 +10633,11 @@
         <v>53327</v>
       </c>
       <c r="F6" s="1"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="9">
         <v>2020</v>
       </c>
@@ -7958,19 +10654,87 @@
         <v>97950</v>
       </c>
       <c r="F7" s="1"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H7">
+        <f>H6*10000</f>
+        <v>90000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
+      <c r="B8" s="10">
+        <f>$H$7</f>
+        <v>90000</v>
+      </c>
+      <c r="C8" s="10">
+        <f t="shared" ref="C8:E8" si="2">$H$7</f>
+        <v>90000</v>
+      </c>
+      <c r="D8" s="10">
+        <f t="shared" si="2"/>
+        <v>90000</v>
+      </c>
+      <c r="E8" s="10">
+        <f t="shared" si="2"/>
+        <v>90000</v>
+      </c>
       <c r="F8" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x14">
+      <controls>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="20481" r:id="rId3" name="Drop Down 1">
+              <controlPr defaultSize="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>15240</xdr:colOff>
+                    <xdr:row>8</xdr:row>
+                    <xdr:rowOff>137160</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>160020</xdr:colOff>
+                    <xdr:row>9</xdr:row>
+                    <xdr:rowOff>152400</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="20482" r:id="rId4" name="Spinner 2">
+              <controlPr defaultSize="0" autoPict="0">
+                <anchor moveWithCells="1" sizeWithCells="1">
+                  <from>
+                    <xdr:col>0</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:row>7</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:row>8</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+      </controls>
+    </mc:Choice>
+  </mc:AlternateContent>
 </worksheet>
 </file>
 
@@ -7990,7 +10754,7 @@
   <sheetData>
     <row r="2" spans="2:9" x14ac:dyDescent="0.3">
       <c r="I2">
-        <v>70</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.3">
@@ -7999,7 +10763,7 @@
       </c>
       <c r="C5" s="12">
         <f>I2*1000</f>
-        <v>70000</v>
+        <v>80000</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.3">
@@ -8016,7 +10780,7 @@
       </c>
       <c r="C7" s="17">
         <f>C5-C6</f>
-        <v>20000</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.3">
@@ -8025,7 +10789,7 @@
       </c>
       <c r="C8" s="18">
         <f>C7/C5</f>
-        <v>0.2857142857142857</v>
+        <v>0.375</v>
       </c>
     </row>
   </sheetData>
@@ -8064,13 +10828,15 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B274C54-6B4F-4330-8F14-86A0AED00443}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B274C54-6B4F-4330-8F14-86A0AED00443}">
   <sheetPr>
     <tabColor theme="7"/>
   </sheetPr>
-  <dimension ref="B5:C8"/>
+  <dimension ref="B2:H8"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -8079,13 +10845,27 @@
     <col min="3" max="3" width="11.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="H2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="H3">
+        <f>H2*1000</f>
+        <v>68000</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B5" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="12"/>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C5" s="12">
+        <f>H3</f>
+        <v>68000</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B6" s="13" t="s">
         <v>8</v>
       </c>
@@ -8093,20 +10873,56 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B7" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="17"/>
-    </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C7" s="17">
+        <f>C5-C6</f>
+        <v>18000</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="18"/>
+      <c r="C8" s="18">
+        <f>C7/C5</f>
+        <v>0.26470588235294118</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x14">
+      <controls>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="21505" r:id="rId3" name="Scroll Bar 1">
+              <controlPr defaultSize="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>15240</xdr:colOff>
+                    <xdr:row>0</xdr:row>
+                    <xdr:rowOff>167640</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:row>3</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+      </controls>
+    </mc:Choice>
+  </mc:AlternateContent>
 </worksheet>
 </file>
 
@@ -8114,7 +10930,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F79FDEB-AA4C-4379-916A-1AA7124428F0}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -8129,7 +10947,7 @@
       </c>
       <c r="C1" s="15">
         <f>COUNTIFS(B2:B11,TRUE)/COUNTA(B2:B11)</f>
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -8169,7 +10987,7 @@
         <v>17</v>
       </c>
       <c r="B6" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>